<commit_message>
Update 12231-9003 Wie oft Internetnutzung_männlich_weiblich.xlsx
</commit_message>
<xml_diff>
--- a/3.Semester/Datenanalyse/12231-9003 Wie oft Internetnutzung_männlich_weiblich.xlsx
+++ b/3.Semester/Datenanalyse/12231-9003 Wie oft Internetnutzung_männlich_weiblich.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Desktop\Studium\3.Semester\Datenanalyse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E390A58C-BE09-454C-93D0-B71CBF2E41C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E05DFF0-416C-4C8A-9DD9-E7EB609DE241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{A9571DE0-E607-40ED-B9E3-4FCBAF959CAF}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -65,7 +65,7 @@
     <t>(Mehrere Elemente)</t>
   </si>
   <si>
-    <t>Summe von value</t>
+    <t>Mittelwert von value</t>
   </si>
 </sst>
 </file>
@@ -3318,12 +3318,53 @@
         <c:marker>
           <c:symbol val="none"/>
         </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
       </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
-        <c:grouping val="stacked"/>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -3399,37 +3440,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>12.6</c:v>
+                  <c:v>6.3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>88.3</c:v>
+                  <c:v>44.15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>99</c:v>
+                  <c:v>49.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>157</c:v>
+                  <c:v>78.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>26</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>38.299999999999997</c:v>
+                  <c:v>19.149999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>74.3</c:v>
+                  <c:v>37.15</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>86.9</c:v>
+                  <c:v>43.45</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>17</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>161</c:v>
+                  <c:v>80.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.4</c:v>
+                  <c:v>4.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3515,37 +3556,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>81.400000000000006</c:v>
+                  <c:v>40.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22.4</c:v>
+                  <c:v>11.2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>86.399999999999991</c:v>
+                  <c:v>43.199999999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>87</c:v>
+                  <c:v>43.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>93.3</c:v>
+                  <c:v>46.65</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>70.599999999999994</c:v>
+                  <c:v>35.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>27</c:v>
+                  <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>93</c:v>
+                  <c:v>46.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>23</c:v>
+                  <c:v>11.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>94.1</c:v>
+                  <c:v>47.05</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3631,37 +3672,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>36.799999999999997</c:v>
+                  <c:v>18.399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>157.19999999999999</c:v>
+                  <c:v>78.599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>166.6</c:v>
+                  <c:v>83.3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>21.3</c:v>
+                  <c:v>10.65</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>88</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>24</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>24.6</c:v>
+                  <c:v>12.3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>85.9</c:v>
+                  <c:v>42.95</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>89</c:v>
+                  <c:v>44.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5301,7 +5342,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EF65A2FC-A92C-4490-BEDD-A3F24959A4B9}" name="PivotTable5" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="13">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EF65A2FC-A92C-4490-BEDD-A3F24959A4B9}" name="PivotTable5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="17">
   <location ref="A3:D16" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" multipleItemSelectionAllowed="1" showAll="0">
@@ -5491,7 +5532,7 @@
     <pageField fld="1" hier="-1"/>
   </pageFields>
   <dataFields count="1">
-    <dataField name="Summe von value" fld="3" baseField="0" baseItem="0"/>
+    <dataField name="Mittelwert von value" fld="3" subtotal="average" baseField="0" baseItem="0"/>
   </dataFields>
   <chartFormats count="16">
     <chartFormat chart="0" format="71" series="1">
@@ -6010,7 +6051,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6075,13 +6116,13 @@
         <v>2006</v>
       </c>
       <c r="B5" s="3">
-        <v>12.6</v>
+        <v>6.3</v>
       </c>
       <c r="C5" s="3">
-        <v>81.400000000000006</v>
+        <v>40.700000000000003</v>
       </c>
       <c r="D5" s="3">
-        <v>36.799999999999997</v>
+        <v>18.399999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -6089,13 +6130,13 @@
         <v>2007</v>
       </c>
       <c r="B6" s="3">
-        <v>88.3</v>
+        <v>44.15</v>
       </c>
       <c r="C6" s="3">
-        <v>21</v>
+        <v>10.5</v>
       </c>
       <c r="D6" s="3">
-        <v>157.19999999999999</v>
+        <v>78.599999999999994</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -6103,13 +6144,13 @@
         <v>2008</v>
       </c>
       <c r="B7" s="3">
-        <v>99</v>
+        <v>49.5</v>
       </c>
       <c r="C7" s="3">
-        <v>22.4</v>
+        <v>11.2</v>
       </c>
       <c r="D7" s="3">
-        <v>24</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -6117,13 +6158,13 @@
         <v>2009</v>
       </c>
       <c r="B8" s="3">
-        <v>157</v>
+        <v>78.5</v>
       </c>
       <c r="C8" s="3">
-        <v>86.399999999999991</v>
+        <v>43.199999999999996</v>
       </c>
       <c r="D8" s="3">
-        <v>166.6</v>
+        <v>83.3</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -6131,13 +6172,13 @@
         <v>2010</v>
       </c>
       <c r="B9" s="3">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C9" s="3">
-        <v>87</v>
+        <v>43.5</v>
       </c>
       <c r="D9" s="3">
-        <v>21.3</v>
+        <v>10.65</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -6145,13 +6186,13 @@
         <v>2011</v>
       </c>
       <c r="B10" s="3">
-        <v>38.299999999999997</v>
+        <v>19.149999999999999</v>
       </c>
       <c r="C10" s="3">
-        <v>93.3</v>
+        <v>46.65</v>
       </c>
       <c r="D10" s="3">
-        <v>88</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -6159,13 +6200,13 @@
         <v>2012</v>
       </c>
       <c r="B11" s="3">
-        <v>74.3</v>
+        <v>37.15</v>
       </c>
       <c r="C11" s="3">
-        <v>70.599999999999994</v>
+        <v>35.299999999999997</v>
       </c>
       <c r="D11" s="3">
-        <v>24</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -6173,13 +6214,13 @@
         <v>2013</v>
       </c>
       <c r="B12" s="3">
-        <v>86.9</v>
+        <v>43.45</v>
       </c>
       <c r="C12" s="3">
-        <v>27</v>
+        <v>13.5</v>
       </c>
       <c r="D12" s="3">
-        <v>24.6</v>
+        <v>12.3</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -6187,13 +6228,13 @@
         <v>2014</v>
       </c>
       <c r="B13" s="3">
-        <v>17</v>
+        <v>8.5</v>
       </c>
       <c r="C13" s="3">
-        <v>93</v>
+        <v>46.5</v>
       </c>
       <c r="D13" s="3">
-        <v>85.9</v>
+        <v>42.95</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -6201,13 +6242,13 @@
         <v>2015</v>
       </c>
       <c r="B14" s="3">
-        <v>161</v>
+        <v>80.5</v>
       </c>
       <c r="C14" s="3">
-        <v>23</v>
+        <v>11.5</v>
       </c>
       <c r="D14" s="3">
-        <v>89</v>
+        <v>44.5</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -6215,13 +6256,13 @@
         <v>2017</v>
       </c>
       <c r="B15" s="3">
-        <v>9.4</v>
+        <v>4.7</v>
       </c>
       <c r="C15" s="3">
-        <v>94.1</v>
+        <v>47.05</v>
       </c>
       <c r="D15" s="3">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -6229,13 +6270,13 @@
         <v>10</v>
       </c>
       <c r="B16" s="3">
-        <v>769.8</v>
+        <v>34.990909090909092</v>
       </c>
       <c r="C16" s="3">
-        <v>699.2</v>
+        <v>31.781818181818185</v>
       </c>
       <c r="D16" s="3">
-        <v>727.40000000000009</v>
+        <v>33.06363636363637</v>
       </c>
     </row>
   </sheetData>
@@ -6248,7 +6289,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A970430-3E0D-4024-8886-7212D0FE6E60}">
   <dimension ref="A1:D111"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>

</xml_diff>